<commit_message>
router + controller + rapport journalier de hier
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport_journalier_Samuel.xlsx
+++ b/rapport journalier/Rapport_journalier_Samuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\cours analyse projet final\mypetsitter\rapport journalier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5755CAB3-84FF-4B1E-B71B-9BD4411D20CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F3649F-7352-4D50-9013-2B68905330A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t xml:space="preserve">DATE : </t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>DATE : 7 aout</t>
+  </si>
+  <si>
+    <t>difficulte avec git pour reccuperer le code de nassim et vice versa</t>
+  </si>
+  <si>
+    <t>controller animal(90%), requete sql pour animal (50%)</t>
+  </si>
+  <si>
+    <t>fin controller animal, controller facture, controller contrat, controller feedback</t>
+  </si>
+  <si>
+    <t>DATE : 10 aout</t>
+  </si>
+  <si>
+    <t>routers animal facture contrat feedback</t>
+  </si>
+  <si>
+    <t>DIFICULTE:Pas beaucoup avancé, je bloque a savoir quoi faire pour la suite, j'ai contacté richard pour de l'aide</t>
+  </si>
+  <si>
+    <t>router + controller fix</t>
+  </si>
+  <si>
+    <t>DATE : Samuel</t>
   </si>
 </sst>
 </file>
@@ -501,8 +525,8 @@
   </sheetPr>
   <dimension ref="B3:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1087,7 +1111,7 @@
       <c r="F83" s="16"/>
       <c r="G83" s="16"/>
       <c r="H83" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I83" s="16"/>
       <c r="J83" s="18"/>
@@ -1159,7 +1183,7 @@
       <c r="F93" s="16"/>
       <c r="G93" s="16"/>
       <c r="H93" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I93" s="16"/>
       <c r="J93" s="18"/>
@@ -1168,6 +1192,9 @@
       <c r="B94" s="19" t="s">
         <v>3</v>
       </c>
+      <c r="C94" t="s">
+        <v>34</v>
+      </c>
       <c r="J94" s="7"/>
     </row>
     <row r="95" spans="2:10" ht="12.75" x14ac:dyDescent="0.35">
@@ -1182,7 +1209,9 @@
       <c r="B97" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C97" s="10"/>
+      <c r="C97" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="D97" s="10"/>
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
@@ -1226,7 +1255,7 @@
       <c r="F103" s="16"/>
       <c r="G103" s="16"/>
       <c r="H103" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I103" s="16"/>
       <c r="J103" s="18"/>
@@ -1234,6 +1263,9 @@
     <row r="104" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B104" s="19" t="s">
         <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>35</v>
       </c>
       <c r="J104" s="7"/>
     </row>
@@ -1283,17 +1315,17 @@
     </row>
     <row r="113" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B113" s="15" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C113" s="16"/>
       <c r="D113" s="16"/>
       <c r="E113" s="17" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F113" s="16"/>
       <c r="G113" s="16"/>
       <c r="H113" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I113" s="16"/>
       <c r="J113" s="18"/>
@@ -1302,6 +1334,9 @@
       <c r="B114" s="19" t="s">
         <v>3</v>
       </c>
+      <c r="C114" t="s">
+        <v>37</v>
+      </c>
       <c r="J114" s="7"/>
     </row>
     <row r="115" spans="2:10" ht="12.75" x14ac:dyDescent="0.35">
@@ -1314,7 +1349,7 @@
     </row>
     <row r="117" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B117" s="20" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="C117" s="10"/>
       <c r="D117" s="10"/>
@@ -1350,17 +1385,17 @@
     </row>
     <row r="123" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B123" s="15" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C123" s="16"/>
       <c r="D123" s="16"/>
       <c r="E123" s="17" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F123" s="16"/>
       <c r="G123" s="16"/>
       <c r="H123" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I123" s="16"/>
       <c r="J123" s="18"/>
@@ -1368,6 +1403,9 @@
     <row r="124" spans="2:10" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B124" s="19" t="s">
         <v>3</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
       </c>
       <c r="J124" s="7"/>
     </row>

</xml_diff>